<commit_message>
review up down excel
</commit_message>
<xml_diff>
--- a/templates/sample-danhmuc-tochuc-demo.xlsx
+++ b/templates/sample-danhmuc-tochuc-demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DINHNV\MyData\LAPTRINH\NODE4\ionic4.qlns\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C6BDFA9-A86B-4667-B74E-100FE193AA92}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CAAA37B-03C6-46A5-A103-067A174A4563}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9105" yWindow="345" windowWidth="14535" windowHeight="12405" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7470" yWindow="690" windowWidth="18330" windowHeight="12405" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="organizations" sheetId="16" r:id="rId1"/>
@@ -365,7 +365,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -393,6 +393,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -496,7 +508,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -528,6 +540,8 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="33" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -543,7 +557,8 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="33" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="33" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="33" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="33" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="34">
     <cellStyle name="20% - Accent2 2" xfId="32" xr:uid="{9CCA8FE9-6B14-409D-8217-A36B47B0E62F}"/>
@@ -925,13 +940,13 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.25" customWidth="1"/>
-    <col min="2" max="2" width="16.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.375" customWidth="1"/>
     <col min="3" max="3" width="9.625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" customWidth="1"/>
     <col min="5" max="5" width="10.125" customWidth="1"/>
@@ -951,22 +966,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
     </row>
     <row r="2" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
       <c r="E2" s="2">
         <v>1</v>
       </c>
@@ -1060,40 +1075,40 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.375" customWidth="1"/>
     <col min="4" max="4" width="27.5" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="8.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.625" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
       <c r="E2" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="63" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -1135,7 +1150,7 @@
       <c r="G4">
         <v>2</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="14" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1158,7 +1173,7 @@
       <c r="G5">
         <v>2</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="14" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1181,7 +1196,7 @@
       <c r="G6">
         <v>2</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="14" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1201,7 +1216,7 @@
       <c r="G7">
         <v>3</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="14" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1224,7 +1239,7 @@
       <c r="G8">
         <v>3</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="14" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1247,7 +1262,7 @@
       <c r="G9">
         <v>3</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="14" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1267,7 +1282,7 @@
       <c r="G10">
         <v>1</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="14" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1290,7 +1305,7 @@
       <c r="G11">
         <v>1</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="14" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1313,7 +1328,7 @@
       <c r="G12">
         <v>1</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" s="14" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1333,7 +1348,7 @@
       <c r="G13">
         <v>4</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13" s="14" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1356,7 +1371,7 @@
       <c r="G14">
         <v>4</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H14" s="14" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1375,45 +1390,49 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="D4" sqref="D4:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.75" customWidth="1"/>
     <col min="4" max="4" width="14.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5" customWidth="1"/>
+    <col min="6" max="6" width="19.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.75" customWidth="1"/>
+    <col min="8" max="8" width="13.125" customWidth="1"/>
+    <col min="9" max="9" width="12.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
       <c r="G1" s="9"/>
       <c r="H1" s="9"/>
       <c r="I1" s="9"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
       <c r="G2" s="10">
         <v>1</v>
       </c>
       <c r="H2" s="9"/>
       <c r="I2" s="9"/>
     </row>
-    <row r="3" spans="1:9" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>0</v>
       </c>
@@ -1452,20 +1471,20 @@
       <c r="C4" s="9">
         <v>1</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="20" t="s">
         <v>50</v>
       </c>
       <c r="E4" s="9">
         <v>8</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="20" t="s">
         <v>32</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="I4" s="9"/>
+      <c r="I4" s="20"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
@@ -1477,20 +1496,20 @@
       <c r="C5" s="9">
         <v>1</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="20" t="s">
         <v>50</v>
       </c>
       <c r="E5" s="9">
         <v>7</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="20" t="s">
         <v>29</v>
       </c>
       <c r="G5" s="9"/>
       <c r="H5" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="I5" s="9"/>
+      <c r="I5" s="20"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
@@ -1502,20 +1521,20 @@
       <c r="C6" s="9">
         <v>2</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="20" t="s">
         <v>9</v>
       </c>
       <c r="E6" s="9">
         <v>1</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="20" t="s">
         <v>20</v>
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="I6" s="9"/>
+      <c r="I6" s="20"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
@@ -1527,20 +1546,20 @@
       <c r="C7" s="9">
         <v>2</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="20" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="9">
         <v>2</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="20" t="s">
         <v>23</v>
       </c>
       <c r="G7" s="9"/>
       <c r="H7" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="I7" s="9"/>
+      <c r="I7" s="20"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
@@ -1552,20 +1571,20 @@
       <c r="C8" s="9">
         <v>3</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="21" t="s">
         <v>64</v>
       </c>
       <c r="E8" s="9">
         <v>4</v>
       </c>
-      <c r="F8" s="18" t="s">
+      <c r="F8" s="21" t="s">
         <v>67</v>
       </c>
       <c r="G8" s="9"/>
       <c r="H8" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="I8" s="9"/>
+      <c r="I8" s="21"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
@@ -1577,20 +1596,20 @@
       <c r="C9" s="9">
         <v>3</v>
       </c>
-      <c r="D9" s="18" t="s">
+      <c r="D9" s="21" t="s">
         <v>64</v>
       </c>
       <c r="E9" s="9">
         <v>5</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="F9" s="21" t="s">
         <v>68</v>
       </c>
       <c r="G9" s="9"/>
       <c r="H9" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="I9" s="9"/>
+      <c r="I9" s="21"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
@@ -1602,20 +1621,20 @@
       <c r="C10" s="9">
         <v>3</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="D10" s="21" t="s">
         <v>64</v>
       </c>
       <c r="E10" s="9">
         <v>6</v>
       </c>
-      <c r="F10" s="18" t="s">
+      <c r="F10" s="21" t="s">
         <v>69</v>
       </c>
       <c r="G10" s="9"/>
       <c r="H10" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="I10" s="9"/>
+      <c r="I10" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
review all and commit to push heroku
</commit_message>
<xml_diff>
--- a/templates/sample-danhmuc-tochuc-demo.xlsx
+++ b/templates/sample-danhmuc-tochuc-demo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DINHNV\MyData\LAPTRINH\NODE4\ionic4.qlns\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CAAA37B-03C6-46A5-A103-067A174A4563}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DDA439B-625A-41AB-8C70-E4C8FC324F2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7470" yWindow="690" windowWidth="18330" windowHeight="12405" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="organizations" sheetId="16" r:id="rId1"/>
@@ -542,6 +542,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="33" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="33" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -557,8 +559,6 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="33" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="33" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="33" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="34">
     <cellStyle name="20% - Accent2 2" xfId="32" xr:uid="{9CCA8FE9-6B14-409D-8217-A36B47B0E62F}"/>
@@ -939,8 +939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{838C49C0-4525-4B19-A798-BE216164A953}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -966,22 +966,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
     </row>
     <row r="2" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
       <c r="E2" s="2">
         <v>1</v>
       </c>
@@ -1090,20 +1090,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
       <c r="E2" s="2">
         <v>1</v>
       </c>
@@ -1389,7 +1389,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{242C06C0-DDA0-461D-A210-41B729E4406C}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4:D10"/>
     </sheetView>
   </sheetViews>
@@ -1405,27 +1405,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
       <c r="G1" s="9"/>
       <c r="H1" s="9"/>
       <c r="I1" s="9"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
       <c r="G2" s="10">
         <v>1</v>
       </c>
@@ -1471,20 +1471,20 @@
       <c r="C4" s="9">
         <v>1</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="15" t="s">
         <v>50</v>
       </c>
       <c r="E4" s="9">
         <v>8</v>
       </c>
-      <c r="F4" s="20" t="s">
+      <c r="F4" s="15" t="s">
         <v>32</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="I4" s="20"/>
+      <c r="I4" s="15"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
@@ -1496,20 +1496,20 @@
       <c r="C5" s="9">
         <v>1</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="15" t="s">
         <v>50</v>
       </c>
       <c r="E5" s="9">
         <v>7</v>
       </c>
-      <c r="F5" s="20" t="s">
+      <c r="F5" s="15" t="s">
         <v>29</v>
       </c>
       <c r="G5" s="9"/>
       <c r="H5" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="I5" s="20"/>
+      <c r="I5" s="15"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
@@ -1521,20 +1521,20 @@
       <c r="C6" s="9">
         <v>2</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="15" t="s">
         <v>9</v>
       </c>
       <c r="E6" s="9">
         <v>1</v>
       </c>
-      <c r="F6" s="20" t="s">
+      <c r="F6" s="15" t="s">
         <v>20</v>
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="I6" s="20"/>
+      <c r="I6" s="15"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
@@ -1546,20 +1546,20 @@
       <c r="C7" s="9">
         <v>2</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="15" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="9">
         <v>2</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="15" t="s">
         <v>23</v>
       </c>
       <c r="G7" s="9"/>
       <c r="H7" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="I7" s="20"/>
+      <c r="I7" s="15"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
@@ -1571,20 +1571,20 @@
       <c r="C8" s="9">
         <v>3</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="16" t="s">
         <v>64</v>
       </c>
       <c r="E8" s="9">
         <v>4</v>
       </c>
-      <c r="F8" s="21" t="s">
+      <c r="F8" s="16" t="s">
         <v>67</v>
       </c>
       <c r="G8" s="9"/>
       <c r="H8" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="I8" s="21"/>
+      <c r="I8" s="16"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
@@ -1596,20 +1596,20 @@
       <c r="C9" s="9">
         <v>3</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="D9" s="16" t="s">
         <v>64</v>
       </c>
       <c r="E9" s="9">
         <v>5</v>
       </c>
-      <c r="F9" s="21" t="s">
+      <c r="F9" s="16" t="s">
         <v>68</v>
       </c>
       <c r="G9" s="9"/>
       <c r="H9" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="I9" s="21"/>
+      <c r="I9" s="16"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
@@ -1621,20 +1621,20 @@
       <c r="C10" s="9">
         <v>3</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="D10" s="16" t="s">
         <v>64</v>
       </c>
       <c r="E10" s="9">
         <v>6</v>
       </c>
-      <c r="F10" s="21" t="s">
+      <c r="F10" s="16" t="s">
         <v>69</v>
       </c>
       <c r="G10" s="9"/>
       <c r="H10" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="I10" s="21"/>
+      <c r="I10" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
review all ok server
</commit_message>
<xml_diff>
--- a/templates/sample-danhmuc-tochuc-demo.xlsx
+++ b/templates/sample-danhmuc-tochuc-demo.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DINHNV\MyData\LAPTRINH\NODE4\ionic4.qlns\templates\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DDA439B-625A-41AB-8C70-E4C8FC324F2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="organizations" sheetId="16" r:id="rId1"/>
     <sheet name="job_roles" sheetId="18" r:id="rId2"/>
     <sheet name="staffs" sheetId="19" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -221,9 +215,6 @@
     <t>Lê Thị Hảo</t>
   </si>
   <si>
-    <t>[4,5,6]</t>
-  </si>
-  <si>
     <t>Phòng Tổng hợp</t>
   </si>
   <si>
@@ -249,12 +240,15 @@
   </si>
   <si>
     <t>Mô tả Trợ lý phòng Tổng hợp</t>
+  </si>
+  <si>
+    <t>[4,5]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
@@ -508,7 +502,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -559,9 +553,10 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="33" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="33" applyFont="1"/>
   </cellXfs>
   <cellStyles count="34">
-    <cellStyle name="20% - Accent2 2" xfId="32" xr:uid="{9CCA8FE9-6B14-409D-8217-A36B47B0E62F}"/>
+    <cellStyle name="20% - Accent2 2" xfId="32"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -589,12 +584,12 @@
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 13 2 2 2 2" xfId="28" xr:uid="{84E13167-2D8D-40CF-A091-58BFDA5A82B5}"/>
-    <cellStyle name="Normal 13 2 2 2 2 2" xfId="29" xr:uid="{0F640A71-A93E-4EA6-B209-195F6B1D713D}"/>
-    <cellStyle name="Normal 2" xfId="33" xr:uid="{4A6ED15C-4C78-4166-8C0D-82B1C82CB0E7}"/>
-    <cellStyle name="Normal 4" xfId="31" xr:uid="{26FC5792-469A-410F-801C-F623F1013E60}"/>
-    <cellStyle name="Normal 6" xfId="27" xr:uid="{BD51DE9F-87D9-4D12-910B-16D23962C238}"/>
-    <cellStyle name="Percent 2" xfId="30" xr:uid="{DCF93D55-E0EF-43EE-84C6-58C701670029}"/>
+    <cellStyle name="Normal 13 2 2 2 2" xfId="28"/>
+    <cellStyle name="Normal 13 2 2 2 2 2" xfId="29"/>
+    <cellStyle name="Normal 2" xfId="33"/>
+    <cellStyle name="Normal 4" xfId="31"/>
+    <cellStyle name="Normal 6" xfId="27"/>
+    <cellStyle name="Percent 2" xfId="30"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -936,10 +931,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{838C49C0-4525-4B19-A798-BE216164A953}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -1031,13 +1026,13 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5" t="s">
         <v>64</v>
-      </c>
-      <c r="C5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D5" t="s">
-        <v>65</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -1071,7 +1066,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{643B1BD3-B5DE-4929-A458-65E1D27E27F1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1205,19 +1200,19 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C7" t="s">
         <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G7">
         <v>3</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1225,13 +1220,13 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C8" t="s">
         <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F8">
         <v>4</v>
@@ -1240,7 +1235,7 @@
         <v>3</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1248,13 +1243,13 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C9" t="s">
         <v>27</v>
       </c>
       <c r="D9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F9">
         <v>4</v>
@@ -1263,7 +1258,7 @@
         <v>3</v>
       </c>
       <c r="H9" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1386,11 +1381,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{242C06C0-DDA0-461D-A210-41B729E4406C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:D10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1572,13 +1567,13 @@
         <v>3</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E8" s="9">
         <v>4</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G8" s="9"/>
       <c r="H8" s="9" t="s">
@@ -1597,13 +1592,13 @@
         <v>3</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E9" s="9">
         <v>5</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G9" s="9"/>
       <c r="H9" s="9" t="s">
@@ -1622,17 +1617,17 @@
         <v>3</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E10" s="9">
         <v>6</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G10" s="9"/>
-      <c r="H10" s="9" t="s">
-        <v>63</v>
+      <c r="H10" s="22" t="s">
+        <v>72</v>
       </c>
       <c r="I10" s="16"/>
     </row>

</xml_diff>